<commit_message>
Añadido, editado y eliminado
AÑADIDO
Nombre Pelicula en tabla pelicula
Asientos Disponibles en Funcion
EDITADO
Nombre en Boleto de tipo a Tipo Persona
Nombre en Detalles venta Boleto de tipo a Tipo Persona
ELIMINADO
Tipo asiento en tabla Sala
</commit_message>
<xml_diff>
--- a/Docs/documentacion.xlsx
+++ b/Docs/documentacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACULTAD\POO\Proyecto Carlos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11E9379-7FC8-4323-8AC4-93DABF261862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEF1C77A-2D21-4D1B-A6C3-CA99DA377F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="11640" tabRatio="170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>Ventas Boletos</t>
   </si>
@@ -39,9 +39,6 @@
     <t>ID Función</t>
   </si>
   <si>
-    <t>Tipo Boleto</t>
-  </si>
-  <si>
     <t>Costo total</t>
   </si>
   <si>
@@ -135,18 +132,12 @@
     <t>ID Película</t>
   </si>
   <si>
-    <t>Tipo Boleto (niño, adulto,etc)</t>
-  </si>
-  <si>
     <t>ID Usuario</t>
   </si>
   <si>
     <t>Asiento</t>
   </si>
   <si>
-    <t>tipo (normal, VIP)</t>
-  </si>
-  <si>
     <t>Pelicula asignada</t>
   </si>
   <si>
@@ -156,9 +147,6 @@
     <t>Num. de sala</t>
   </si>
   <si>
-    <t>Tipo de asientos</t>
-  </si>
-  <si>
     <t>Cantidad de asientos</t>
   </si>
   <si>
@@ -210,14 +198,29 @@
     <t>contraseña</t>
   </si>
   <si>
-    <t>nivel</t>
+    <t>Tipo Persona</t>
+  </si>
+  <si>
+    <t>Tipo Persona (niño, adulto,etc)</t>
+  </si>
+  <si>
+    <t>Num Sala</t>
+  </si>
+  <si>
+    <t>Asientos Disponibles.</t>
+  </si>
+  <si>
+    <t>ID_Funcion</t>
+  </si>
+  <si>
+    <t>Nombre Pelicula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -236,8 +239,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +286,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -370,6 +385,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,71 +708,71 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="2.28515625" customWidth="1"/>
-    <col min="4" max="4" width="2.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="2.33203125" customWidth="1"/>
+    <col min="4" max="4" width="2.5546875" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
+    <col min="11" max="11" width="2.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="D1" s="18"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="17"/>
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="17"/>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -762,333 +781,334 @@
       </c>
       <c r="D4" s="17"/>
       <c r="F4" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" s="17"/>
       <c r="F5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="17"/>
       <c r="F6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="J6" s="23"/>
       <c r="L6" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="17"/>
       <c r="J7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="17"/>
       <c r="F8" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="17"/>
       <c r="F9" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>8</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D10" s="17"/>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>9</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D11" s="17"/>
-      <c r="F11" s="1" t="s">
-        <v>36</v>
+      <c r="F11" s="23" t="s">
+        <v>58</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="17"/>
       <c r="F12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>11</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D13" s="17"/>
       <c r="F13" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>12</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="17"/>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>13</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="17"/>
       <c r="F15" s="14" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16" s="17"/>
       <c r="F16" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D17" s="17"/>
       <c r="F17" s="7"/>
       <c r="H17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D18" s="17"/>
       <c r="F18" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D19" s="17"/>
       <c r="F19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D20" s="17"/>
-      <c r="F20" s="1" t="s">
-        <v>4</v>
+      <c r="F20" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D21" s="17"/>
       <c r="F21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="17"/>
       <c r="F22" s="1" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="17"/>
       <c r="F23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="17"/>
       <c r="H24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D25" s="17"/>
       <c r="F25" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="J25" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="17"/>
       <c r="F26" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="17"/>
       <c r="F27" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D28" s="17"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>

</xml_diff>